<commit_message>
add validation import v1
</commit_message>
<xml_diff>
--- a/public/import/reporforium.xlsx
+++ b/public/import/reporforium.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zakky\Downloads\akta\akta\public\import\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zakky\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3EBC44E-4202-48C0-B31D-AA976A061849}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1614D14A-055F-45BF-A300-A4E3179E2DFB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{995F4D5A-BA8D-4227-9043-0DAB9C7FA8C6}"/>
   </bookViews>
@@ -51,13 +51,13 @@
     <t>Sifat Akta</t>
   </si>
   <si>
-    <t>SK Kemenhumkam</t>
-  </si>
-  <si>
     <t>Nama Penghadap</t>
   </si>
   <si>
     <t>zakky taufiqurrohman,andi,kiki,paijo,imin</t>
+  </si>
+  <si>
+    <t>SK Kemenhumham</t>
   </si>
 </sst>
 </file>
@@ -447,7 +447,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -455,7 +455,7 @@
     <col min="2" max="2" width="14.42578125" customWidth="1"/>
     <col min="3" max="3" width="15.85546875" customWidth="1"/>
     <col min="4" max="4" width="18.28515625" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" customWidth="1"/>
     <col min="6" max="6" width="21.140625" customWidth="1"/>
     <col min="7" max="7" width="41.7109375" customWidth="1"/>
     <col min="8" max="8" width="37.7109375" customWidth="1"/>
@@ -475,10 +475,10 @@
         <v>7</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>9</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>3</v>
@@ -486,7 +486,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1211</v>
+        <v>12323</v>
       </c>
       <c r="B2">
         <v>12</v>
@@ -501,7 +501,7 @@
         <v>2</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G2" t="s">
         <v>0</v>

</xml_diff>